<commit_message>
added the datatable interview question and string interview question along with excel dependency
</commit_message>
<xml_diff>
--- a/Salary.xlsx
+++ b/Salary.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sachin\Documents\UiPath\Pratice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20F8AA3F-52BE-493D-B12E-E3A340E5F5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0237559-4ADA-4C09-A493-37C8242E98A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FCAA5692-D3C3-406A-ABF4-6FA6EE01DFD7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{FCAA5692-D3C3-406A-ABF4-6FA6EE01DFD7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ActualOutput" sheetId="7" r:id="rId1"/>
+    <sheet name="Output" sheetId="6" r:id="rId2"/>
+    <sheet name="Employee" sheetId="1" r:id="rId3"/>
+    <sheet name="Department" sheetId="2" r:id="rId4"/>
+    <sheet name="RequiredOutput" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,6 +37,56 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="15">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>salary</t>
+  </si>
+  <si>
+    <t>departmentid</t>
+  </si>
+  <si>
+    <t>Sachin</t>
+  </si>
+  <si>
+    <t>Paresh</t>
+  </si>
+  <si>
+    <t>Gaurav</t>
+  </si>
+  <si>
+    <t>Trisha</t>
+  </si>
+  <si>
+    <t>Tushar</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>departmentname</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -66,8 +120,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,13 +438,344 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C406336-0326-4B93-A91E-709B2586141A}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D9B5D3-645F-40E6-B9BC-2998F98238F0}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>80000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7043D1D6-2508-4EF3-95D2-0D44263D1DAB}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>90000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C406336-0326-4B93-A91E-709B2586141A}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>70000</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>90000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>80000</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1">
+        <v>60000</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>90000</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA1D88F-058C-4BB4-80CC-8AF6A9433595}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C85ACB-7A9E-48EE-BF9F-48C7962A8E40}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>80000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>